<commit_message>
clean up before transfer to CDPH
</commit_message>
<xml_diff>
--- a/Inputs/CAcounties.xlsx
+++ b/Inputs/CAcounties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshua/Documents/GitHub/LEMMA-Forecasts2/Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F5D940-CFDD-4547-9419-530B7D551406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E63DF3-DAD1-7B48-B6CA-7BBF6E890ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,22 +630,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1528,53 +1528,53 @@
   <sheetData>
     <row r="1" spans="1:13" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="37" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38" t="s">
+      <c r="I1" s="39"/>
+      <c r="J1" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38" t="s">
+      <c r="K1" s="36"/>
+      <c r="L1" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="M1" s="38"/>
+      <c r="M1" s="36"/>
     </row>
     <row r="2" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="17"/>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36" t="s">
+      <c r="C2" s="40"/>
+      <c r="D2" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="36"/>
-      <c r="F2" s="39" t="s">
+      <c r="E2" s="40"/>
+      <c r="F2" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="36" t="s">
+      <c r="G2" s="38"/>
+      <c r="H2" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="36"/>
-      <c r="J2" s="39" t="s">
+      <c r="I2" s="40"/>
+      <c r="J2" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="40"/>
+      <c r="K2" s="38"/>
       <c r="L2" s="18" t="s">
         <v>57</v>
       </c>
@@ -1785,17 +1785,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="H2:I2"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A43:A487 A5:A36" xr:uid="{DFFBA6CA-6EEC-F54F-9268-B981437AD2EB}">
@@ -1941,7 +1941,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2044,7 +2044,7 @@
         <v>81</v>
       </c>
       <c r="B8" s="3">
-        <v>2000</v>
+        <v>400</v>
       </c>
       <c r="C8" s="1">
         <v>4000</v>
@@ -2055,7 +2055,7 @@
         <v>84</v>
       </c>
       <c r="B9" s="3">
-        <v>1000</v>
+        <v>200</v>
       </c>
       <c r="C9" s="1">
         <v>2000</v>

</xml_diff>